<commit_message>
add file size to indicator meta
</commit_message>
<xml_diff>
--- a/docs/indicator_search.xlsx
+++ b/docs/indicator_search.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccmothes\Desktop\NASA-prison-EJ\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8CEFA3-88E9-4831-B0F7-D7B73B469435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4702B2DD-1014-43B7-950D-7C5E095031B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="420" windowWidth="17280" windowHeight="9030" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
+    <workbookView xWindow="-23340" yWindow="1425" windowWidth="20040" windowHeight="12975" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>indicator</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>file_format</t>
+  </si>
+  <si>
+    <t>file_size</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E86D84-176C-47AA-8351-F9BBDD699BE6}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,11 +427,12 @@
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,12 +449,15 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
filled out indicator search
</commit_message>
<xml_diff>
--- a/docs/indicator_search.xlsx
+++ b/docs/indicator_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccmothes\Desktop\NASA-prison-EJ\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\Desktop\CSU\Geospatial Centroid\NASA-prison-EJ\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4702B2DD-1014-43B7-950D-7C5E095031B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABE3E82-30CF-4002-ADCA-C8F1730723CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23340" yWindow="1425" windowWidth="20040" windowHeight="12975" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
+    <workbookView xWindow="4380" yWindow="2100" windowWidth="17280" windowHeight="9420" xr2:uid="{592A012E-B0BA-4FE2-858A-16360FC85FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
   <si>
     <t>indicator</t>
   </si>
@@ -63,16 +63,285 @@
   </si>
   <si>
     <t>file_size</t>
+  </si>
+  <si>
+    <t>Heat Index</t>
+  </si>
+  <si>
+    <t>Tree Canopy Cover</t>
+  </si>
+  <si>
+    <t>CONUS</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>CONUS, AK, HI</t>
+  </si>
+  <si>
+    <t>30m</t>
+  </si>
+  <si>
+    <t>~11.5GB</t>
+  </si>
+  <si>
+    <t>USDA</t>
+  </si>
+  <si>
+    <t>https://data.fs.usda.gov/geodata/rastergateway/treecanopycover/#table1</t>
+  </si>
+  <si>
+    <t>.vat (Value Table)</t>
+  </si>
+  <si>
+    <t>2016 tree canopy cover raster published in 2019. Analytical version with calculated cover values</t>
+  </si>
+  <si>
+    <t>Wildfire Risk</t>
+  </si>
+  <si>
+    <t>Flood Risk</t>
+  </si>
+  <si>
+    <t>Ozone</t>
+  </si>
+  <si>
+    <t>PM 2.5</t>
+  </si>
+  <si>
+    <t>Traffic Density</t>
+  </si>
+  <si>
+    <t>Pesticide Use</t>
+  </si>
+  <si>
+    <t>Superfund</t>
+  </si>
+  <si>
+    <t>Nuclear Power Plants</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://cds.climate.copernicus.eu/cdsapp#!/dataset/satellite-ozone?tab=form</t>
+  </si>
+  <si>
+    <t>Copernicus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFO: https://www.usgs.gov/landsat-missions/landsat-collection-2-level-3-burned-area-science-product, DATA: </t>
+  </si>
+  <si>
+    <t>.TIF</t>
+  </si>
+  <si>
+    <t>NASA NOAA-20</t>
+  </si>
+  <si>
+    <t>RAW instrument data</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>.h5</t>
+  </si>
+  <si>
+    <t>https://ozoneaq.gsfc.nasa.gov/data/omps/#prods=149</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>.gdb</t>
+  </si>
+  <si>
+    <t>~13.5GB</t>
+  </si>
+  <si>
+    <t>FEMA</t>
+  </si>
+  <si>
+    <t>https://gis.fema.gov/NFHL/NFHL_Key_Layers.gdb.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full geodatabase </t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>.csv</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Census tract level</t>
+  </si>
+  <si>
+    <t>CDC</t>
+  </si>
+  <si>
+    <t>https://data.cdc.gov/Environmental-Health-Toxicology/Daily-Census-Tract-Level-PM2-5-Concentrations-2016/7vu4-ngxx/data</t>
+  </si>
+  <si>
+    <t>EarthExplorer</t>
+  </si>
+  <si>
+    <t>PM 2.5 and Ozone</t>
+  </si>
+  <si>
+    <t>48MB</t>
+  </si>
+  <si>
+    <t>https://data.cdc.gov/Environmental-Health-Toxicology/Air-Quality-Measures-on-the-National-Environmental/cjae-szjv</t>
+  </si>
+  <si>
+    <t>Countains a variety of ozone and PM statistics per year</t>
+  </si>
+  <si>
+    <t>.txt</t>
+  </si>
+  <si>
+    <t>64.43MB</t>
+  </si>
+  <si>
+    <t>USGS ScienceBase</t>
+  </si>
+  <si>
+    <t>https://www.sciencebase.gov/catalog/item/5e95c12282ce172707f2524e</t>
+  </si>
+  <si>
+    <t>2013 to 2017 data</t>
+  </si>
+  <si>
+    <t>Lat., Long.</t>
+  </si>
+  <si>
+    <t>.PDF</t>
+  </si>
+  <si>
+    <t>&lt;1GB</t>
+  </si>
+  <si>
+    <t>EPA</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/superfund/superfund-data-and-reports</t>
+  </si>
+  <si>
+    <t>Superfunds to exist in HI, AK, other dataset contains such</t>
+  </si>
+  <si>
+    <t>Superfund, ATSDR</t>
+  </si>
+  <si>
+    <t>Site Polygons</t>
+  </si>
+  <si>
+    <t>.shp</t>
+  </si>
+  <si>
+    <t>NASA SEDAC</t>
+  </si>
+  <si>
+    <t>https://sedac.ciesin.columbia.edu/data/collection/superfund</t>
+  </si>
+  <si>
+    <t>GeoTIFF</t>
+  </si>
+  <si>
+    <t>0.01 degrees</t>
+  </si>
+  <si>
+    <t>https://sedac.ciesin.columbia.edu/data/set/sdei-global-annual-gwr-pm2-5-modis-misr-seawifs-aod-v4-gl-03/data-download</t>
+  </si>
+  <si>
+    <t>Yearly data from 1998 to 2019</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/tmas-2020</t>
+  </si>
+  <si>
+    <t>Federal Highway Administration</t>
+  </si>
+  <si>
+    <t>.shp, .csv</t>
+  </si>
+  <si>
+    <t>~1MB</t>
+  </si>
+  <si>
+    <t>https://sedac.ciesin.columbia.edu/data/set/energy-pop-exposure-nuclear-plants-locations</t>
+  </si>
+  <si>
+    <t>Last Updated 2012</t>
+  </si>
+  <si>
+    <t>~4MB</t>
+  </si>
+  <si>
+    <t>World Resources Institute</t>
+  </si>
+  <si>
+    <t>https://datasets.wri.org/dataset/globalpowerplantdatabase</t>
+  </si>
+  <si>
+    <t>Updated June 2021, includes nuclear power</t>
+  </si>
+  <si>
+    <t>All Power Plants</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/earth-engine/datasets/catalog/LANDSAT_LC08_C02_T2_L2#description</t>
+  </si>
+  <si>
+    <t>Earth Engine</t>
+  </si>
+  <si>
+    <t>Landsat 8 data collection. Can be filtered to any timeseries</t>
+  </si>
+  <si>
+    <t>USGS (Google Earth Engine)</t>
+  </si>
+  <si>
+    <t>1000m</t>
+  </si>
+  <si>
+    <t>NASA (Google Earth Engine)</t>
+  </si>
+  <si>
+    <t>MOD11A1 LST</t>
+  </si>
+  <si>
+    <t>Landsat 8 OLI LST</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/earth-engine/datasets/catalog/MODIS_061_MOD11A1#description</t>
+  </si>
+  <si>
+    <t>Daily global Land Surface Temperature. Potentially more easy and efficient to work with.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,13 +364,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,25 +686,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E86D84-176C-47AA-8351-F9BBDD699BE6}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +733,423 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H8" r:id="rId1" location="prods=149" xr:uid="{F264A2DB-1619-4E2C-84AD-32F894EAA961}"/>
+    <hyperlink ref="H4" r:id="rId2" location="description" xr:uid="{EECA4D4F-8922-4C5E-9EA6-1B7D81F7A1CA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>